<commit_message>
changed the gui language & added gui components
</commit_message>
<xml_diff>
--- a/S9+.xlsx
+++ b/S9+.xlsx
@@ -1,37 +1,105 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a6edeb39450ad7f9/Dokumente/Github/Amazon-Price-Tracker/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_8B6895B787F495745AF806637F39DD29E609A330" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{75DE9307-369C-4861-AE35-83ECA448A1C0}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Preis</t>
+  </si>
+  <si>
+    <t>Datum</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy S9+ Smartphone (6,2 Zoll (15,7cm) 64GB interner Speicher, Dual SIM) - Deutsche Version</t>
+  </si>
+  <si>
+    <t>661,73 €</t>
+  </si>
+  <si>
+    <t>10-10-2019 19:16:28</t>
+  </si>
+  <si>
+    <t>10-10-2019 19:35:10</t>
+  </si>
+  <si>
+    <t>661,68 €</t>
+  </si>
+  <si>
+    <t>10-10-2019 19:39:22</t>
+  </si>
+  <si>
+    <t>586,81 €</t>
+  </si>
+  <si>
+    <t>14-11-2019 10:46:45</t>
+  </si>
+  <si>
+    <t>14-11-2019 10:48:05</t>
+  </si>
+  <si>
+    <t>14-11-2019 10:48:14</t>
+  </si>
+  <si>
+    <t>586,80 €</t>
+  </si>
+  <si>
+    <t>14-11-2019 10:48:21</t>
+  </si>
+  <si>
+    <t>14-11-2019 10:48:29</t>
+  </si>
+  <si>
+    <t>599,99 €</t>
+  </si>
+  <si>
+    <t>12-12-2019 10:31:43</t>
+  </si>
+  <si>
+    <t>12-12-2019 10:31:53</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,26 +114,43 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -353,173 +438,138 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="34.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Preis</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Datum</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Samsung Galaxy S9+ Smartphone (6,2 Zoll (15,7cm) 64GB interner Speicher, Dual SIM) - Deutsche Version</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>661,73 €</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>10-10-2019 19:16:28</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Samsung Galaxy S9+ Smartphone (6,2 Zoll (15,7cm) 64GB interner Speicher, Dual SIM) - Deutsche Version</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>661,73 €</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>10-10-2019 19:35:10</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Samsung Galaxy S9+ Smartphone (6,2 Zoll (15,7cm) 64GB interner Speicher, Dual SIM) - Deutsche Version</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>661,68 €</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>10-10-2019 19:39:22</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Samsung Galaxy S9+ Smartphone (6,2 Zoll (15,7cm) 64GB interner Speicher, Dual SIM) - Deutsche Version</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>586,81 €</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>14-11-2019 10:46:45</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Samsung Galaxy S9+ Smartphone (6,2 Zoll (15,7cm) 64GB interner Speicher, Dual SIM) - Deutsche Version</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>586,81 €</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>14-11-2019 10:48:05</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Samsung Galaxy S9+ Smartphone (6,2 Zoll (15,7cm) 64GB interner Speicher, Dual SIM) - Deutsche Version</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>586,81 €</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>14-11-2019 10:48:14</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Samsung Galaxy S9+ Smartphone (6,2 Zoll (15,7cm) 64GB interner Speicher, Dual SIM) - Deutsche Version</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>586,80 €</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>14-11-2019 10:48:21</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Samsung Galaxy S9+ Smartphone (6,2 Zoll (15,7cm) 64GB interner Speicher, Dual SIM) - Deutsche Version</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>586,80 €</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>14-11-2019 10:48:29</t>
-        </is>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>